<commit_message>
support import multi datasheet
</commit_message>
<xml_diff>
--- a/test/import.xlsx
+++ b/test/import.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13740" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13740" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="基础数据导入表" sheetId="1" r:id="rId1"/>
-    <sheet name="选项" sheetId="2" r:id="rId2"/>
+    <sheet name="aquatic_region" sheetId="3" r:id="rId2"/>
+    <sheet name="选项" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
   <si>
     <t>类目表</t>
   </si>
@@ -235,6 +236,37 @@
   </si>
   <si>
     <t>类目编号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>is_home</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EP</t>
+  </si>
+  <si>
+    <t>中国</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>进口</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -377,8 +409,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="83">
+  <cellStyleXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -489,7 +523,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="83">
+  <cellStyles count="85">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -531,6 +565,7 @@
     <cellStyle name="超链接" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
@@ -572,6 +607,7 @@
     <cellStyle name="访问过的超链接" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -903,7 +939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
+    <sheetView topLeftCell="C2" workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
@@ -1100,12 +1136,6 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>选项!C2:C15</xm:f>
-          </x14:formula1>
-          <xm:sqref>I4:I104</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
             <xm:f>选项!$D$2:$D$3</xm:f>
           </x14:formula1>
           <xm:sqref>K4:K56</xm:sqref>
@@ -1115,6 +1145,12 @@
             <xm:f>选项!$E$2:$E$3</xm:f>
           </x14:formula1>
           <xm:sqref>J4:J127</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>选项!C2:C15</xm:f>
+          </x14:formula1>
+          <xm:sqref>I4:I104</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1126,6 +1162,64 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:F15"/>
   <sheetViews>

</xml_diff>